<commit_message>
IMC-621 Local Charges Inserter, simplify rate_basis handling
Former-commit-id: dacaea0b3aa614176877f3b818a041b5d0eba68c
</commit_message>
<xml_diff>
--- a/app/classes/data_reader/__fakedata/normanglobal__local_charges.xlsx
+++ b/app/classes/data_reader/__fakedata/normanglobal__local_charges.xlsx
@@ -403,8 +403,8 @@
   </sheetPr>
   <dimension ref="A1:AC415"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AC2" activeCellId="0" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -539,7 +539,7 @@
       </c>
       <c r="C2" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>43465</v>
@@ -629,7 +629,7 @@
       </c>
       <c r="C3" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>43465</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="C4" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>43465</v>
@@ -809,7 +809,7 @@
       </c>
       <c r="C5" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>43465</v>
@@ -899,7 +899,7 @@
       </c>
       <c r="C6" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>43465</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="C7" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>43465</v>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="C8" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>43465</v>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="C9" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>43465</v>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C10" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>43465</v>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="C11" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>43465</v>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C12" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>43465</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="C13" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>43465</v>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="C14" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>43465</v>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="C15" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>43465</v>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="C16" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>43465</v>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="C17" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>43465</v>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="C18" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>43465</v>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="C19" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>43465</v>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="C20" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D20" s="4" t="n">
         <v>43465</v>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="C21" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>43465</v>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="C22" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>43465</v>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="C23" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>43465</v>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="C24" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D24" s="4" t="n">
         <v>43465</v>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="C25" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D25" s="4" t="n">
         <v>43465</v>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="C26" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>43465</v>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="C27" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D27" s="4" t="n">
         <v>43465</v>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="C28" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>43465</v>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="C29" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>43465</v>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="C30" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>43465</v>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="C31" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>43465</v>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="C32" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D32" s="4" t="n">
         <v>43465</v>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="C33" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D33" s="4" t="n">
         <v>43465</v>
@@ -3415,7 +3415,7 @@
       </c>
       <c r="C34" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D34" s="4" t="n">
         <v>43465</v>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="C35" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>43465</v>
@@ -3595,7 +3595,7 @@
       </c>
       <c r="C36" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D36" s="4" t="n">
         <v>43465</v>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="C37" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D37" s="4" t="n">
         <v>43465</v>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="C38" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D38" s="4" t="n">
         <v>43465</v>
@@ -3865,7 +3865,7 @@
       </c>
       <c r="C39" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D39" s="4" t="n">
         <v>43465</v>
@@ -3955,7 +3955,7 @@
       </c>
       <c r="C40" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D40" s="4" t="n">
         <v>43465</v>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="C41" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D41" s="4" t="n">
         <v>43465</v>
@@ -4135,7 +4135,7 @@
       </c>
       <c r="C42" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D42" s="4" t="n">
         <v>43465</v>
@@ -4225,7 +4225,7 @@
       </c>
       <c r="C43" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D43" s="4" t="n">
         <v>43465</v>
@@ -4315,7 +4315,7 @@
       </c>
       <c r="C44" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D44" s="4" t="n">
         <v>43465</v>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="C45" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>43465</v>
@@ -4495,7 +4495,7 @@
       </c>
       <c r="C46" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D46" s="4" t="n">
         <v>43465</v>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="C47" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>43465</v>
@@ -4675,7 +4675,7 @@
       </c>
       <c r="C48" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D48" s="4" t="n">
         <v>43465</v>
@@ -4765,7 +4765,7 @@
       </c>
       <c r="C49" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D49" s="4" t="n">
         <v>43465</v>
@@ -4855,7 +4855,7 @@
       </c>
       <c r="C50" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D50" s="4" t="n">
         <v>43465</v>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="C51" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D51" s="4" t="n">
         <v>43465</v>
@@ -5035,7 +5035,7 @@
       </c>
       <c r="C52" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D52" s="4" t="n">
         <v>43465</v>
@@ -5125,7 +5125,7 @@
       </c>
       <c r="C53" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D53" s="4" t="n">
         <v>43465</v>
@@ -5215,7 +5215,7 @@
       </c>
       <c r="C54" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>43465</v>
@@ -5303,7 +5303,7 @@
       </c>
       <c r="C55" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D55" s="4" t="n">
         <v>43465</v>
@@ -5393,7 +5393,7 @@
       </c>
       <c r="C56" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>43465</v>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="C57" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D57" s="4" t="n">
         <v>43465</v>
@@ -5573,7 +5573,7 @@
       </c>
       <c r="C58" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D58" s="4" t="n">
         <v>43465</v>
@@ -5663,7 +5663,7 @@
       </c>
       <c r="C59" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>43465</v>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="C60" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D60" s="4" t="n">
         <v>43465</v>
@@ -5843,7 +5843,7 @@
       </c>
       <c r="C61" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D61" s="4" t="n">
         <v>43465</v>
@@ -5933,7 +5933,7 @@
       </c>
       <c r="C62" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D62" s="4" t="n">
         <v>43465</v>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="C63" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D63" s="4" t="n">
         <v>43465</v>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="C64" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D64" s="4" t="n">
         <v>43465</v>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="C65" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D65" s="4" t="n">
         <v>43465</v>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="C66" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D66" s="4" t="n">
         <v>43465</v>
@@ -6383,7 +6383,7 @@
       </c>
       <c r="C67" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D67" s="4" t="n">
         <v>43465</v>
@@ -6473,7 +6473,7 @@
       </c>
       <c r="C68" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D68" s="4" t="n">
         <v>43465</v>
@@ -6563,7 +6563,7 @@
       </c>
       <c r="C69" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D69" s="4" t="n">
         <v>43465</v>
@@ -6653,7 +6653,7 @@
       </c>
       <c r="C70" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D70" s="4" t="n">
         <v>43465</v>
@@ -6743,7 +6743,7 @@
       </c>
       <c r="C71" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D71" s="4" t="n">
         <v>43465</v>
@@ -6833,7 +6833,7 @@
       </c>
       <c r="C72" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D72" s="4" t="n">
         <v>43465</v>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="C73" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D73" s="4" t="n">
         <v>43465</v>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="C74" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D74" s="4" t="n">
         <v>43465</v>
@@ -7103,7 +7103,7 @@
       </c>
       <c r="C75" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D75" s="4" t="n">
         <v>43465</v>
@@ -7193,7 +7193,7 @@
       </c>
       <c r="C76" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D76" s="4" t="n">
         <v>43465</v>
@@ -7283,7 +7283,7 @@
       </c>
       <c r="C77" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D77" s="4" t="n">
         <v>43465</v>
@@ -7373,7 +7373,7 @@
       </c>
       <c r="C78" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D78" s="4" t="n">
         <v>43465</v>
@@ -7461,7 +7461,7 @@
       </c>
       <c r="C79" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D79" s="4" t="n">
         <v>43465</v>
@@ -7551,7 +7551,7 @@
       </c>
       <c r="C80" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D80" s="4" t="n">
         <v>43465</v>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="C81" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D81" s="4" t="n">
         <v>43465</v>
@@ -7731,7 +7731,7 @@
       </c>
       <c r="C82" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D82" s="4" t="n">
         <v>43465</v>
@@ -7821,7 +7821,7 @@
       </c>
       <c r="C83" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D83" s="4" t="n">
         <v>43465</v>
@@ -7911,7 +7911,7 @@
       </c>
       <c r="C84" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D84" s="4" t="n">
         <v>43465</v>
@@ -8001,7 +8001,7 @@
       </c>
       <c r="C85" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D85" s="4" t="n">
         <v>43465</v>
@@ -8091,7 +8091,7 @@
       </c>
       <c r="C86" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D86" s="4" t="n">
         <v>43465</v>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="C87" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D87" s="4" t="n">
         <v>43465</v>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="C88" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D88" s="4" t="n">
         <v>43465</v>
@@ -8361,7 +8361,7 @@
       </c>
       <c r="C89" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D89" s="4" t="n">
         <v>43465</v>
@@ -8451,7 +8451,7 @@
       </c>
       <c r="C90" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D90" s="4" t="n">
         <v>43465</v>
@@ -8541,7 +8541,7 @@
       </c>
       <c r="C91" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D91" s="4" t="n">
         <v>43465</v>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="C92" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D92" s="4" t="n">
         <v>43465</v>
@@ -8721,7 +8721,7 @@
       </c>
       <c r="C93" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D93" s="4" t="n">
         <v>43465</v>
@@ -8811,7 +8811,7 @@
       </c>
       <c r="C94" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D94" s="4" t="n">
         <v>43465</v>
@@ -8901,7 +8901,7 @@
       </c>
       <c r="C95" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D95" s="4" t="n">
         <v>43465</v>
@@ -8991,7 +8991,7 @@
       </c>
       <c r="C96" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D96" s="4" t="n">
         <v>43465</v>
@@ -9081,7 +9081,7 @@
       </c>
       <c r="C97" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D97" s="4" t="n">
         <v>43465</v>
@@ -9171,7 +9171,7 @@
       </c>
       <c r="C98" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D98" s="4" t="n">
         <v>43465</v>
@@ -9259,7 +9259,7 @@
       </c>
       <c r="C99" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D99" s="4" t="n">
         <v>43465</v>
@@ -9349,7 +9349,7 @@
       </c>
       <c r="C100" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D100" s="4" t="n">
         <v>43465</v>
@@ -9439,7 +9439,7 @@
       </c>
       <c r="C101" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D101" s="4" t="n">
         <v>43465</v>
@@ -9529,7 +9529,7 @@
       </c>
       <c r="C102" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D102" s="4" t="n">
         <v>43465</v>
@@ -9619,7 +9619,7 @@
       </c>
       <c r="C103" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D103" s="4" t="n">
         <v>43465</v>
@@ -9709,7 +9709,7 @@
       </c>
       <c r="C104" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D104" s="4" t="n">
         <v>43465</v>
@@ -9799,7 +9799,7 @@
       </c>
       <c r="C105" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D105" s="4" t="n">
         <v>43465</v>
@@ -9887,7 +9887,7 @@
       </c>
       <c r="C106" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D106" s="4" t="n">
         <v>43465</v>
@@ -9975,7 +9975,7 @@
       </c>
       <c r="C107" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D107" s="4" t="n">
         <v>43465</v>
@@ -10063,7 +10063,7 @@
       </c>
       <c r="C108" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D108" s="4" t="n">
         <v>43465</v>
@@ -10151,7 +10151,7 @@
       </c>
       <c r="C109" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D109" s="4" t="n">
         <v>43465</v>
@@ -10239,7 +10239,7 @@
       </c>
       <c r="C110" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D110" s="4" t="n">
         <v>43465</v>
@@ -10327,7 +10327,7 @@
       </c>
       <c r="C111" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D111" s="4" t="n">
         <v>43465</v>
@@ -10415,7 +10415,7 @@
       </c>
       <c r="C112" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D112" s="4" t="n">
         <v>43465</v>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="C113" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D113" s="4" t="n">
         <v>43465</v>
@@ -10591,7 +10591,7 @@
       </c>
       <c r="C114" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D114" s="4" t="n">
         <v>43465</v>
@@ -10679,7 +10679,7 @@
       </c>
       <c r="C115" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D115" s="4" t="n">
         <v>43465</v>
@@ -10767,7 +10767,7 @@
       </c>
       <c r="C116" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D116" s="4" t="n">
         <v>43465</v>
@@ -10855,7 +10855,7 @@
       </c>
       <c r="C117" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D117" s="4" t="n">
         <v>43465</v>
@@ -10943,7 +10943,7 @@
       </c>
       <c r="C118" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D118" s="4" t="n">
         <v>43465</v>
@@ -11031,7 +11031,7 @@
       </c>
       <c r="C119" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D119" s="4" t="n">
         <v>43465</v>
@@ -11119,7 +11119,7 @@
       </c>
       <c r="C120" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D120" s="4" t="n">
         <v>43465</v>
@@ -11207,7 +11207,7 @@
       </c>
       <c r="C121" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D121" s="4" t="n">
         <v>43465</v>
@@ -11295,7 +11295,7 @@
       </c>
       <c r="C122" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D122" s="4" t="n">
         <v>43465</v>
@@ -11383,7 +11383,7 @@
       </c>
       <c r="C123" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D123" s="4" t="n">
         <v>43465</v>
@@ -11471,7 +11471,7 @@
       </c>
       <c r="C124" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D124" s="4" t="n">
         <v>43465</v>
@@ -11559,7 +11559,7 @@
       </c>
       <c r="C125" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D125" s="4" t="n">
         <v>43465</v>
@@ -11647,7 +11647,7 @@
       </c>
       <c r="C126" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D126" s="4" t="n">
         <v>43465</v>
@@ -11735,7 +11735,7 @@
       </c>
       <c r="C127" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D127" s="4" t="n">
         <v>43465</v>
@@ -11823,7 +11823,7 @@
       </c>
       <c r="C128" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D128" s="4" t="n">
         <v>43465</v>
@@ -11911,7 +11911,7 @@
       </c>
       <c r="C129" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D129" s="4" t="n">
         <v>43465</v>
@@ -11999,7 +11999,7 @@
       </c>
       <c r="C130" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D130" s="4" t="n">
         <v>43465</v>
@@ -12087,7 +12087,7 @@
       </c>
       <c r="C131" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D131" s="4" t="n">
         <v>43465</v>
@@ -12175,7 +12175,7 @@
       </c>
       <c r="C132" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D132" s="4" t="n">
         <v>43465</v>
@@ -12263,7 +12263,7 @@
       </c>
       <c r="C133" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D133" s="4" t="n">
         <v>43465</v>
@@ -12351,7 +12351,7 @@
       </c>
       <c r="C134" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D134" s="4" t="n">
         <v>43465</v>
@@ -12439,7 +12439,7 @@
       </c>
       <c r="C135" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D135" s="4" t="n">
         <v>43465</v>
@@ -12527,7 +12527,7 @@
       </c>
       <c r="C136" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D136" s="4" t="n">
         <v>43465</v>
@@ -12615,7 +12615,7 @@
       </c>
       <c r="C137" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D137" s="4" t="n">
         <v>43465</v>
@@ -12703,7 +12703,7 @@
       </c>
       <c r="C138" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D138" s="4" t="n">
         <v>43465</v>
@@ -12791,7 +12791,7 @@
       </c>
       <c r="C139" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D139" s="4" t="n">
         <v>43465</v>
@@ -12879,7 +12879,7 @@
       </c>
       <c r="C140" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D140" s="4" t="n">
         <v>43465</v>
@@ -12967,7 +12967,7 @@
       </c>
       <c r="C141" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D141" s="4" t="n">
         <v>43465</v>
@@ -13055,7 +13055,7 @@
       </c>
       <c r="C142" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D142" s="4" t="n">
         <v>43465</v>
@@ -13143,7 +13143,7 @@
       </c>
       <c r="C143" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D143" s="4" t="n">
         <v>43465</v>
@@ -13231,7 +13231,7 @@
       </c>
       <c r="C144" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D144" s="4" t="n">
         <v>43465</v>
@@ -13319,7 +13319,7 @@
       </c>
       <c r="C145" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D145" s="4" t="n">
         <v>43465</v>
@@ -13407,7 +13407,7 @@
       </c>
       <c r="C146" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D146" s="4" t="n">
         <v>43465</v>
@@ -13495,7 +13495,7 @@
       </c>
       <c r="C147" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D147" s="4" t="n">
         <v>43465</v>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="C148" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D148" s="4" t="n">
         <v>43465</v>
@@ -13671,7 +13671,7 @@
       </c>
       <c r="C149" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D149" s="4" t="n">
         <v>43465</v>
@@ -13759,7 +13759,7 @@
       </c>
       <c r="C150" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D150" s="4" t="n">
         <v>43465</v>
@@ -13847,7 +13847,7 @@
       </c>
       <c r="C151" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D151" s="4" t="n">
         <v>43465</v>
@@ -13935,7 +13935,7 @@
       </c>
       <c r="C152" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D152" s="4" t="n">
         <v>43465</v>
@@ -14023,7 +14023,7 @@
       </c>
       <c r="C153" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D153" s="4" t="n">
         <v>43465</v>
@@ -14111,7 +14111,7 @@
       </c>
       <c r="C154" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D154" s="4" t="n">
         <v>43465</v>
@@ -14199,7 +14199,7 @@
       </c>
       <c r="C155" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D155" s="4" t="n">
         <v>43465</v>
@@ -14287,7 +14287,7 @@
       </c>
       <c r="C156" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D156" s="4" t="n">
         <v>43465</v>
@@ -14375,7 +14375,7 @@
       </c>
       <c r="C157" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D157" s="4" t="n">
         <v>43465</v>
@@ -14463,7 +14463,7 @@
       </c>
       <c r="C158" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D158" s="4" t="n">
         <v>43465</v>
@@ -14551,7 +14551,7 @@
       </c>
       <c r="C159" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D159" s="4" t="n">
         <v>43465</v>
@@ -14639,7 +14639,7 @@
       </c>
       <c r="C160" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D160" s="4" t="n">
         <v>43465</v>
@@ -14727,7 +14727,7 @@
       </c>
       <c r="C161" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D161" s="4" t="n">
         <v>43465</v>
@@ -14815,7 +14815,7 @@
       </c>
       <c r="C162" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D162" s="4" t="n">
         <v>43465</v>
@@ -14903,7 +14903,7 @@
       </c>
       <c r="C163" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D163" s="4" t="n">
         <v>43465</v>
@@ -14991,7 +14991,7 @@
       </c>
       <c r="C164" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D164" s="4" t="n">
         <v>43465</v>
@@ -15079,7 +15079,7 @@
       </c>
       <c r="C165" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D165" s="4" t="n">
         <v>43465</v>
@@ -15167,7 +15167,7 @@
       </c>
       <c r="C166" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D166" s="4" t="n">
         <v>43465</v>
@@ -15255,7 +15255,7 @@
       </c>
       <c r="C167" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D167" s="4" t="n">
         <v>43465</v>
@@ -15343,7 +15343,7 @@
       </c>
       <c r="C168" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D168" s="4" t="n">
         <v>43465</v>
@@ -15431,7 +15431,7 @@
       </c>
       <c r="C169" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D169" s="4" t="n">
         <v>43465</v>
@@ -15519,7 +15519,7 @@
       </c>
       <c r="C170" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D170" s="4" t="n">
         <v>43465</v>
@@ -15607,7 +15607,7 @@
       </c>
       <c r="C171" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D171" s="4" t="n">
         <v>43465</v>
@@ -15695,7 +15695,7 @@
       </c>
       <c r="C172" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D172" s="4" t="n">
         <v>43465</v>
@@ -15783,7 +15783,7 @@
       </c>
       <c r="C173" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D173" s="4" t="n">
         <v>43465</v>
@@ -15871,7 +15871,7 @@
       </c>
       <c r="C174" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D174" s="4" t="n">
         <v>43465</v>
@@ -15959,7 +15959,7 @@
       </c>
       <c r="C175" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D175" s="4" t="n">
         <v>43465</v>
@@ -16047,7 +16047,7 @@
       </c>
       <c r="C176" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D176" s="4" t="n">
         <v>43465</v>
@@ -16135,7 +16135,7 @@
       </c>
       <c r="C177" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D177" s="4" t="n">
         <v>43465</v>
@@ -16223,7 +16223,7 @@
       </c>
       <c r="C178" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D178" s="4" t="n">
         <v>43465</v>
@@ -16311,7 +16311,7 @@
       </c>
       <c r="C179" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D179" s="4" t="n">
         <v>43465</v>
@@ -16399,7 +16399,7 @@
       </c>
       <c r="C180" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D180" s="4" t="n">
         <v>43465</v>
@@ -16487,7 +16487,7 @@
       </c>
       <c r="C181" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D181" s="4" t="n">
         <v>43465</v>
@@ -16575,7 +16575,7 @@
       </c>
       <c r="C182" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D182" s="4" t="n">
         <v>43465</v>
@@ -16663,7 +16663,7 @@
       </c>
       <c r="C183" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D183" s="4" t="n">
         <v>43465</v>
@@ -16751,7 +16751,7 @@
       </c>
       <c r="C184" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D184" s="4" t="n">
         <v>43465</v>
@@ -16839,7 +16839,7 @@
       </c>
       <c r="C185" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D185" s="4" t="n">
         <v>43465</v>
@@ -16927,7 +16927,7 @@
       </c>
       <c r="C186" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D186" s="4" t="n">
         <v>43465</v>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="C187" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D187" s="4" t="n">
         <v>43465</v>
@@ -17103,7 +17103,7 @@
       </c>
       <c r="C188" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D188" s="4" t="n">
         <v>43465</v>
@@ -17191,7 +17191,7 @@
       </c>
       <c r="C189" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D189" s="4" t="n">
         <v>43465</v>
@@ -17279,7 +17279,7 @@
       </c>
       <c r="C190" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D190" s="4" t="n">
         <v>43465</v>
@@ -17367,7 +17367,7 @@
       </c>
       <c r="C191" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D191" s="4" t="n">
         <v>43465</v>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="C192" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D192" s="4" t="n">
         <v>43465</v>
@@ -17543,7 +17543,7 @@
       </c>
       <c r="C193" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D193" s="4" t="n">
         <v>43465</v>
@@ -17631,7 +17631,7 @@
       </c>
       <c r="C194" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D194" s="4" t="n">
         <v>43465</v>
@@ -17719,7 +17719,7 @@
       </c>
       <c r="C195" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D195" s="4" t="n">
         <v>43465</v>
@@ -17807,7 +17807,7 @@
       </c>
       <c r="C196" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D196" s="4" t="n">
         <v>43465</v>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="C197" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D197" s="4" t="n">
         <v>43465</v>
@@ -17983,7 +17983,7 @@
       </c>
       <c r="C198" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D198" s="4" t="n">
         <v>43465</v>
@@ -18071,7 +18071,7 @@
       </c>
       <c r="C199" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D199" s="4" t="n">
         <v>43465</v>
@@ -18159,7 +18159,7 @@
       </c>
       <c r="C200" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D200" s="4" t="n">
         <v>43465</v>
@@ -18247,7 +18247,7 @@
       </c>
       <c r="C201" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D201" s="4" t="n">
         <v>43465</v>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="C202" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D202" s="4" t="n">
         <v>43465</v>
@@ -18423,7 +18423,7 @@
       </c>
       <c r="C203" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D203" s="4" t="n">
         <v>43465</v>
@@ -18511,7 +18511,7 @@
       </c>
       <c r="C204" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D204" s="4" t="n">
         <v>43465</v>
@@ -18599,7 +18599,7 @@
       </c>
       <c r="C205" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D205" s="4" t="n">
         <v>43465</v>
@@ -18687,7 +18687,7 @@
       </c>
       <c r="C206" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D206" s="4" t="n">
         <v>43465</v>
@@ -18775,7 +18775,7 @@
       </c>
       <c r="C207" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D207" s="4" t="n">
         <v>43465</v>
@@ -18863,7 +18863,7 @@
       </c>
       <c r="C208" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D208" s="4" t="n">
         <v>43465</v>
@@ -18951,7 +18951,7 @@
       </c>
       <c r="C209" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D209" s="4" t="n">
         <v>43465</v>
@@ -19039,7 +19039,7 @@
       </c>
       <c r="C210" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D210" s="4" t="n">
         <v>43465</v>
@@ -19127,7 +19127,7 @@
       </c>
       <c r="C211" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D211" s="4" t="n">
         <v>43465</v>
@@ -19215,7 +19215,7 @@
       </c>
       <c r="C212" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D212" s="4" t="n">
         <v>43465</v>
@@ -19303,7 +19303,7 @@
       </c>
       <c r="C213" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D213" s="4" t="n">
         <v>43465</v>
@@ -19391,7 +19391,7 @@
       </c>
       <c r="C214" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43420</v>
+        <v>43424</v>
       </c>
       <c r="D214" s="4" t="n">
         <v>43465</v>

</xml_diff>

<commit_message>
IMC-621 Local Charges Inserter, inserting correctly
Former-commit-id: 8c76a8ee5aa86cc0a7b53ebe6b68f9beddde81e3
</commit_message>
<xml_diff>
--- a/app/classes/data_reader/__fakedata/normanglobal__local_charges.xlsx
+++ b/app/classes/data_reader/__fakedata/normanglobal__local_charges.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="China Port " sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'China Port '!$A$1:$AC$203</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5253" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5253" uniqueCount="81">
   <si>
     <t xml:space="preserve">PORT</t>
   </si>
@@ -160,7 +163,7 @@
     <t xml:space="preserve">Port charge</t>
   </si>
   <si>
-    <t xml:space="preserve">CUST</t>
+    <t xml:space="preserve">EXP</t>
   </si>
   <si>
     <t xml:space="preserve">Customs Clearance</t>
@@ -209,6 +212,9 @@
   </si>
   <si>
     <t xml:space="preserve">PER_CBM_TON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUST</t>
   </si>
   <si>
     <t xml:space="preserve">HAN</t>
@@ -270,7 +276,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -313,12 +319,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,10 +388,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -411,8 +407,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G36" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N59" activeCellId="0" sqref="N59:N71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -548,7 +544,7 @@
       </c>
       <c r="C2" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>43465</v>
@@ -638,7 +634,7 @@
       </c>
       <c r="C3" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>43465</v>
@@ -728,7 +724,7 @@
       </c>
       <c r="C4" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>43465</v>
@@ -818,7 +814,7 @@
       </c>
       <c r="C5" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>43465</v>
@@ -908,7 +904,7 @@
       </c>
       <c r="C6" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D6" s="4" t="n">
         <v>43465</v>
@@ -998,7 +994,7 @@
       </c>
       <c r="C7" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D7" s="4" t="n">
         <v>43465</v>
@@ -1088,7 +1084,7 @@
       </c>
       <c r="C8" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D8" s="4" t="n">
         <v>43465</v>
@@ -1178,7 +1174,7 @@
       </c>
       <c r="C9" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>43465</v>
@@ -1268,7 +1264,7 @@
       </c>
       <c r="C10" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>43465</v>
@@ -1358,7 +1354,7 @@
       </c>
       <c r="C11" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D11" s="4" t="n">
         <v>43465</v>
@@ -1448,7 +1444,7 @@
       </c>
       <c r="C12" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>43465</v>
@@ -1538,7 +1534,7 @@
       </c>
       <c r="C13" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D13" s="4" t="n">
         <v>43465</v>
@@ -1628,7 +1624,7 @@
       </c>
       <c r="C14" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D14" s="4" t="n">
         <v>43465</v>
@@ -1718,7 +1714,7 @@
       </c>
       <c r="C15" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D15" s="4" t="n">
         <v>43465</v>
@@ -1808,7 +1804,7 @@
       </c>
       <c r="C16" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D16" s="4" t="n">
         <v>43465</v>
@@ -1898,7 +1894,7 @@
       </c>
       <c r="C17" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>43465</v>
@@ -1988,7 +1984,7 @@
       </c>
       <c r="C18" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D18" s="4" t="n">
         <v>43465</v>
@@ -2078,7 +2074,7 @@
       </c>
       <c r="C19" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D19" s="4" t="n">
         <v>43465</v>
@@ -2096,7 +2092,7 @@
         <v>31</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>47</v>
@@ -2168,7 +2164,7 @@
       </c>
       <c r="C20" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D20" s="4" t="n">
         <v>43465</v>
@@ -2258,7 +2254,7 @@
       </c>
       <c r="C21" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D21" s="4" t="n">
         <v>43465</v>
@@ -2348,7 +2344,7 @@
       </c>
       <c r="C22" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D22" s="4" t="n">
         <v>43465</v>
@@ -2366,10 +2362,10 @@
         <v>31</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>34</v>
@@ -2438,7 +2434,7 @@
       </c>
       <c r="C23" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D23" s="4" t="n">
         <v>43465</v>
@@ -2528,7 +2524,7 @@
       </c>
       <c r="C24" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D24" s="4" t="n">
         <v>43465</v>
@@ -2611,14 +2607,14 @@
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C25" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D25" s="4" t="n">
         <v>43465</v>
@@ -2701,14 +2697,14 @@
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D26" s="4" t="n">
         <v>43465</v>
@@ -2791,14 +2787,14 @@
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D27" s="4" t="n">
         <v>43465</v>
@@ -2881,14 +2877,14 @@
     </row>
     <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D28" s="4" t="n">
         <v>43465</v>
@@ -2971,14 +2967,14 @@
     </row>
     <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D29" s="4" t="n">
         <v>43465</v>
@@ -3061,14 +3057,14 @@
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D30" s="4" t="n">
         <v>43465</v>
@@ -3151,14 +3147,14 @@
     </row>
     <row r="31" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D31" s="4" t="n">
         <v>43465</v>
@@ -3241,14 +3237,14 @@
     </row>
     <row r="32" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D32" s="4" t="n">
         <v>43465</v>
@@ -3331,14 +3327,14 @@
     </row>
     <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D33" s="4" t="n">
         <v>43465</v>
@@ -3421,14 +3417,14 @@
     </row>
     <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D34" s="4" t="n">
         <v>43465</v>
@@ -3511,14 +3507,14 @@
     </row>
     <row r="35" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C35" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D35" s="4" t="n">
         <v>43465</v>
@@ -3601,14 +3597,14 @@
     </row>
     <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C36" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D36" s="4" t="n">
         <v>43465</v>
@@ -3691,14 +3687,14 @@
     </row>
     <row r="37" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D37" s="4" t="n">
         <v>43465</v>
@@ -3781,14 +3777,14 @@
     </row>
     <row r="38" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D38" s="4" t="n">
         <v>43465</v>
@@ -3871,35 +3867,35 @@
     </row>
     <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <f aca="true">TODAY()</f>
+        <v>43425</v>
+      </c>
+      <c r="D39" s="4" t="n">
+        <v>43465</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J39" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="4" t="n">
-        <f aca="true">TODAY()</f>
-        <v>43424</v>
-      </c>
-      <c r="D39" s="4" t="n">
-        <v>43465</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="K39" s="3" t="s">
         <v>34</v>
@@ -3961,14 +3957,14 @@
     </row>
     <row r="40" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D40" s="4" t="n">
         <v>43465</v>
@@ -4051,14 +4047,14 @@
     </row>
     <row r="41" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C41" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D41" s="4" t="n">
         <v>43465</v>
@@ -4076,7 +4072,7 @@
         <v>31</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>47</v>
@@ -4141,14 +4137,14 @@
     </row>
     <row r="42" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D42" s="4" t="n">
         <v>43465</v>
@@ -4231,14 +4227,14 @@
     </row>
     <row r="43" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C43" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D43" s="4" t="n">
         <v>43465</v>
@@ -4321,35 +4317,35 @@
     </row>
     <row r="44" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="4" t="n">
+        <f aca="true">TODAY()</f>
+        <v>43425</v>
+      </c>
+      <c r="D44" s="4" t="n">
+        <v>43465</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J44" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="4" t="n">
-        <f aca="true">TODAY()</f>
-        <v>43424</v>
-      </c>
-      <c r="D44" s="4" t="n">
-        <v>43465</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="K44" s="3" t="s">
         <v>34</v>
@@ -4411,14 +4407,14 @@
     </row>
     <row r="45" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C45" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D45" s="4" t="n">
         <v>43465</v>
@@ -4501,14 +4497,14 @@
     </row>
     <row r="46" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C46" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D46" s="4" t="n">
         <v>43465</v>
@@ -4526,10 +4522,10 @@
         <v>31</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>34</v>
@@ -4591,14 +4587,14 @@
     </row>
     <row r="47" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C47" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D47" s="4" t="n">
         <v>43465</v>
@@ -4681,14 +4677,14 @@
     </row>
     <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D48" s="4" t="n">
         <v>43465</v>
@@ -4771,14 +4767,14 @@
     </row>
     <row r="49" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C49" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D49" s="4" t="n">
         <v>43465</v>
@@ -4861,14 +4857,14 @@
     </row>
     <row r="50" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C50" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D50" s="4" t="n">
         <v>43465</v>
@@ -4951,14 +4947,14 @@
     </row>
     <row r="51" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C51" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D51" s="4" t="n">
         <v>43465</v>
@@ -5041,14 +5037,14 @@
     </row>
     <row r="52" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C52" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D52" s="4" t="n">
         <v>43465</v>
@@ -5131,14 +5127,14 @@
     </row>
     <row r="53" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C53" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D53" s="4" t="n">
         <v>43465</v>
@@ -5156,7 +5152,7 @@
         <v>31</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>47</v>
@@ -5221,14 +5217,14 @@
     </row>
     <row r="54" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C54" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D54" s="4" t="n">
         <v>43465</v>
@@ -5311,14 +5307,14 @@
     </row>
     <row r="55" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C55" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D55" s="4" t="n">
         <v>43465</v>
@@ -5401,14 +5397,14 @@
     </row>
     <row r="56" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C56" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D56" s="4" t="n">
         <v>43465</v>
@@ -5426,10 +5422,10 @@
         <v>31</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K56" s="3" t="s">
         <v>34</v>
@@ -5491,35 +5487,35 @@
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="4" t="n">
+        <f aca="true">TODAY()</f>
+        <v>43425</v>
+      </c>
+      <c r="D57" s="4" t="n">
+        <v>43465</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J57" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57" s="4" t="n">
-        <f aca="true">TODAY()</f>
-        <v>43424</v>
-      </c>
-      <c r="D57" s="4" t="n">
-        <v>43465</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="K57" s="3" t="s">
         <v>34</v>
@@ -5581,14 +5577,14 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C58" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D58" s="4" t="n">
         <v>43465</v>
@@ -5621,7 +5617,7 @@
         <v>36</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O58" s="3" t="s">
         <v>50</v>
@@ -5671,14 +5667,14 @@
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C59" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D59" s="4" t="n">
         <v>43465</v>
@@ -5711,7 +5707,7 @@
         <v>36</v>
       </c>
       <c r="N59" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O59" s="3" t="s">
         <v>41</v>
@@ -5761,14 +5757,14 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C60" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D60" s="4" t="n">
         <v>43465</v>
@@ -5801,7 +5797,7 @@
         <v>36</v>
       </c>
       <c r="N60" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O60" s="3" t="s">
         <v>41</v>
@@ -5851,14 +5847,14 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C61" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D61" s="4" t="n">
         <v>43465</v>
@@ -5891,7 +5887,7 @@
         <v>36</v>
       </c>
       <c r="N61" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O61" s="3" t="s">
         <v>41</v>
@@ -5941,14 +5937,14 @@
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C62" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D62" s="4" t="n">
         <v>43465</v>
@@ -5981,7 +5977,7 @@
         <v>36</v>
       </c>
       <c r="N62" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O62" s="3" t="s">
         <v>50</v>
@@ -6031,14 +6027,14 @@
     </row>
     <row r="63" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C63" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D63" s="4" t="n">
         <v>43465</v>
@@ -6071,7 +6067,7 @@
         <v>36</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O63" s="3" t="s">
         <v>50</v>
@@ -6121,14 +6117,14 @@
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C64" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D64" s="4" t="n">
         <v>43465</v>
@@ -6149,7 +6145,7 @@
         <v>56</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>34</v>
@@ -6161,7 +6157,7 @@
         <v>36</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O64" s="3" t="s">
         <v>50</v>
@@ -6211,14 +6207,14 @@
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C65" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D65" s="4" t="n">
         <v>43465</v>
@@ -6251,7 +6247,7 @@
         <v>36</v>
       </c>
       <c r="N65" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O65" s="3" t="s">
         <v>41</v>
@@ -6301,14 +6297,14 @@
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C66" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D66" s="4" t="n">
         <v>43465</v>
@@ -6341,7 +6337,7 @@
         <v>36</v>
       </c>
       <c r="N66" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O66" s="3" t="s">
         <v>62</v>
@@ -6391,14 +6387,14 @@
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C67" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D67" s="4" t="n">
         <v>43465</v>
@@ -6431,7 +6427,7 @@
         <v>36</v>
       </c>
       <c r="N67" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O67" s="3" t="s">
         <v>50</v>
@@ -6481,14 +6477,14 @@
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C68" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D68" s="4" t="n">
         <v>43465</v>
@@ -6521,7 +6517,7 @@
         <v>36</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O68" s="3" t="s">
         <v>50</v>
@@ -6571,14 +6567,14 @@
     </row>
     <row r="69" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C69" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D69" s="4" t="n">
         <v>43465</v>
@@ -6596,10 +6592,10 @@
         <v>31</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K69" s="3" t="s">
         <v>34</v>
@@ -6611,7 +6607,7 @@
         <v>36</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O69" s="3" t="s">
         <v>50</v>
@@ -6661,14 +6657,14 @@
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C70" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D70" s="4" t="n">
         <v>43465</v>
@@ -6701,7 +6697,7 @@
         <v>36</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O70" s="3" t="s">
         <v>50</v>
@@ -6751,14 +6747,14 @@
     </row>
     <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C71" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D71" s="4" t="n">
         <v>43465</v>
@@ -6776,10 +6772,10 @@
         <v>31</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>34</v>
@@ -6791,7 +6787,7 @@
         <v>36</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O71" s="3" t="s">
         <v>38</v>
@@ -6841,14 +6837,14 @@
     </row>
     <row r="72" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C72" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D72" s="4" t="n">
         <v>43465</v>
@@ -6931,14 +6927,14 @@
     </row>
     <row r="73" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C73" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D73" s="4" t="n">
         <v>43465</v>
@@ -7021,14 +7017,14 @@
     </row>
     <row r="74" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C74" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D74" s="4" t="n">
         <v>43465</v>
@@ -7111,14 +7107,14 @@
     </row>
     <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C75" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D75" s="4" t="n">
         <v>43465</v>
@@ -7201,14 +7197,14 @@
     </row>
     <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C76" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D76" s="4" t="n">
         <v>43465</v>
@@ -7291,14 +7287,14 @@
     </row>
     <row r="77" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C77" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D77" s="4" t="n">
         <v>43465</v>
@@ -7381,14 +7377,14 @@
     </row>
     <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C78" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D78" s="4" t="n">
         <v>43465</v>
@@ -7471,14 +7467,14 @@
     </row>
     <row r="79" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C79" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D79" s="4" t="n">
         <v>43465</v>
@@ -7561,14 +7557,14 @@
     </row>
     <row r="80" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C80" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D80" s="4" t="n">
         <v>43465</v>
@@ -7651,14 +7647,14 @@
     </row>
     <row r="81" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C81" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D81" s="4" t="n">
         <v>43465</v>
@@ -7741,14 +7737,14 @@
     </row>
     <row r="82" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C82" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D82" s="4" t="n">
         <v>43465</v>
@@ -7831,14 +7827,14 @@
     </row>
     <row r="83" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C83" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D83" s="4" t="n">
         <v>43465</v>
@@ -7921,14 +7917,14 @@
     </row>
     <row r="84" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C84" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D84" s="4" t="n">
         <v>43465</v>
@@ -8011,14 +8007,14 @@
     </row>
     <row r="85" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C85" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D85" s="4" t="n">
         <v>43465</v>
@@ -8036,7 +8032,7 @@
         <v>31</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>47</v>
@@ -8101,14 +8097,14 @@
     </row>
     <row r="86" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C86" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D86" s="4" t="n">
         <v>43465</v>
@@ -8191,14 +8187,14 @@
     </row>
     <row r="87" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C87" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D87" s="4" t="n">
         <v>43465</v>
@@ -8281,14 +8277,14 @@
     </row>
     <row r="88" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C88" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D88" s="4" t="n">
         <v>43465</v>
@@ -8306,10 +8302,10 @@
         <v>31</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K88" s="3" t="s">
         <v>34</v>
@@ -8371,14 +8367,14 @@
     </row>
     <row r="89" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C89" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D89" s="4" t="n">
         <v>43465</v>
@@ -8461,14 +8457,14 @@
     </row>
     <row r="90" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C90" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D90" s="4" t="n">
         <v>43465</v>
@@ -8551,14 +8547,14 @@
     </row>
     <row r="91" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C91" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D91" s="4" t="n">
         <v>43465</v>
@@ -8641,14 +8637,14 @@
     </row>
     <row r="92" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C92" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D92" s="4" t="n">
         <v>43465</v>
@@ -8731,14 +8727,14 @@
     </row>
     <row r="93" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C93" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D93" s="4" t="n">
         <v>43465</v>
@@ -8821,14 +8817,14 @@
     </row>
     <row r="94" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C94" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D94" s="4" t="n">
         <v>43465</v>
@@ -8911,14 +8907,14 @@
     </row>
     <row r="95" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C95" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D95" s="4" t="n">
         <v>43465</v>
@@ -9001,14 +8997,14 @@
     </row>
     <row r="96" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C96" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D96" s="4" t="n">
         <v>43465</v>
@@ -9091,14 +9087,14 @@
     </row>
     <row r="97" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C97" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D97" s="4" t="n">
         <v>43465</v>
@@ -9181,14 +9177,14 @@
     </row>
     <row r="98" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C98" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D98" s="4" t="n">
         <v>43465</v>
@@ -9271,14 +9267,14 @@
     </row>
     <row r="99" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C99" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D99" s="4" t="n">
         <v>43465</v>
@@ -9361,14 +9357,14 @@
     </row>
     <row r="100" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C100" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D100" s="4" t="n">
         <v>43465</v>
@@ -9451,14 +9447,14 @@
     </row>
     <row r="101" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C101" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D101" s="4" t="n">
         <v>43465</v>
@@ -9541,14 +9537,14 @@
     </row>
     <row r="102" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C102" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D102" s="4" t="n">
         <v>43465</v>
@@ -9631,14 +9627,14 @@
     </row>
     <row r="103" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C103" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D103" s="4" t="n">
         <v>43465</v>
@@ -9721,14 +9717,14 @@
     </row>
     <row r="104" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C104" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D104" s="4" t="n">
         <v>43465</v>
@@ -9811,14 +9807,14 @@
     </row>
     <row r="105" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C105" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D105" s="4" t="n">
         <v>43465</v>
@@ -9836,7 +9832,7 @@
         <v>31</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>47</v>
@@ -9901,14 +9897,14 @@
     </row>
     <row r="106" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C106" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D106" s="4" t="n">
         <v>43465</v>
@@ -9991,14 +9987,14 @@
     </row>
     <row r="107" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C107" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D107" s="4" t="n">
         <v>43465</v>
@@ -10081,14 +10077,14 @@
     </row>
     <row r="108" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C108" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D108" s="4" t="n">
         <v>43465</v>
@@ -10106,10 +10102,10 @@
         <v>31</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K108" s="3" t="s">
         <v>34</v>
@@ -10171,14 +10167,14 @@
     </row>
     <row r="109" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C109" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D109" s="4" t="n">
         <v>43465</v>
@@ -10261,14 +10257,14 @@
     </row>
     <row r="110" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C110" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D110" s="4" t="n">
         <v>43465</v>
@@ -10351,14 +10347,14 @@
     </row>
     <row r="111" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B111" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C111" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D111" s="4" t="n">
         <v>43465</v>
@@ -10441,14 +10437,14 @@
     </row>
     <row r="112" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B112" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C112" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D112" s="4" t="n">
         <v>43465</v>
@@ -10531,14 +10527,14 @@
     </row>
     <row r="113" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C113" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D113" s="4" t="n">
         <v>43465</v>
@@ -10621,14 +10617,14 @@
     </row>
     <row r="114" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C114" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D114" s="4" t="n">
         <v>43465</v>
@@ -10711,14 +10707,14 @@
     </row>
     <row r="115" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B115" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C115" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D115" s="4" t="n">
         <v>43465</v>
@@ -10801,14 +10797,14 @@
     </row>
     <row r="116" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C116" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D116" s="4" t="n">
         <v>43465</v>
@@ -10891,14 +10887,14 @@
     </row>
     <row r="117" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C117" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D117" s="4" t="n">
         <v>43465</v>
@@ -10981,14 +10977,14 @@
     </row>
     <row r="118" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C118" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D118" s="4" t="n">
         <v>43465</v>
@@ -11071,14 +11067,14 @@
     </row>
     <row r="119" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C119" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D119" s="4" t="n">
         <v>43465</v>
@@ -11161,14 +11157,14 @@
     </row>
     <row r="120" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C120" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D120" s="4" t="n">
         <v>43465</v>
@@ -11251,14 +11247,14 @@
     </row>
     <row r="121" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B121" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C121" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D121" s="4" t="n">
         <v>43465</v>
@@ -11279,7 +11275,7 @@
         <v>58</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="K121" s="3" t="s">
         <v>34</v>
@@ -11341,14 +11337,14 @@
     </row>
     <row r="122" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C122" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D122" s="4" t="n">
         <v>43465</v>
@@ -11431,14 +11427,14 @@
     </row>
     <row r="123" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B123" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C123" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D123" s="4" t="n">
         <v>43465</v>
@@ -11456,7 +11452,7 @@
         <v>31</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J123" s="3" t="s">
         <v>47</v>
@@ -11521,14 +11517,14 @@
     </row>
     <row r="124" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C124" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D124" s="4" t="n">
         <v>43465</v>
@@ -11611,14 +11607,14 @@
     </row>
     <row r="125" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B125" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C125" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D125" s="4" t="n">
         <v>43465</v>
@@ -11701,14 +11697,14 @@
     </row>
     <row r="126" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B126" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C126" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D126" s="4" t="n">
         <v>43465</v>
@@ -11791,14 +11787,14 @@
     </row>
     <row r="127" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C127" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D127" s="4" t="n">
         <v>43465</v>
@@ -11881,14 +11877,14 @@
     </row>
     <row r="128" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C128" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D128" s="4" t="n">
         <v>43465</v>
@@ -11971,14 +11967,14 @@
     </row>
     <row r="129" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C129" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D129" s="4" t="n">
         <v>43465</v>
@@ -12061,14 +12057,14 @@
     </row>
     <row r="130" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C130" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D130" s="4" t="n">
         <v>43465</v>
@@ -12151,14 +12147,14 @@
     </row>
     <row r="131" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C131" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D131" s="4" t="n">
         <v>43465</v>
@@ -12241,14 +12237,14 @@
     </row>
     <row r="132" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C132" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D132" s="4" t="n">
         <v>43465</v>
@@ -12331,14 +12327,14 @@
     </row>
     <row r="133" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C133" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D133" s="4" t="n">
         <v>43465</v>
@@ -12421,14 +12417,14 @@
     </row>
     <row r="134" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C134" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D134" s="4" t="n">
         <v>43465</v>
@@ -12446,7 +12442,7 @@
         <v>31</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J134" s="3" t="s">
         <v>47</v>
@@ -12511,14 +12507,14 @@
     </row>
     <row r="135" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B135" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C135" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D135" s="4" t="n">
         <v>43465</v>
@@ -12601,14 +12597,14 @@
     </row>
     <row r="136" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B136" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C136" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D136" s="4" t="n">
         <v>43465</v>
@@ -12691,14 +12687,14 @@
     </row>
     <row r="137" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B137" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C137" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D137" s="4" t="n">
         <v>43465</v>
@@ -12716,10 +12712,10 @@
         <v>31</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J137" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K137" s="3" t="s">
         <v>34</v>
@@ -12781,14 +12777,14 @@
     </row>
     <row r="138" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B138" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C138" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D138" s="4" t="n">
         <v>43465</v>
@@ -12806,10 +12802,10 @@
         <v>31</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K138" s="3" t="s">
         <v>34</v>
@@ -12871,14 +12867,14 @@
     </row>
     <row r="139" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B139" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C139" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D139" s="4" t="n">
         <v>43465</v>
@@ -12961,14 +12957,14 @@
     </row>
     <row r="140" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B140" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C140" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D140" s="4" t="n">
         <v>43465</v>
@@ -13051,14 +13047,14 @@
     </row>
     <row r="141" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B141" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C141" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D141" s="4" t="n">
         <v>43465</v>
@@ -13141,14 +13137,14 @@
     </row>
     <row r="142" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B142" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C142" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D142" s="4" t="n">
         <v>43465</v>
@@ -13231,14 +13227,14 @@
     </row>
     <row r="143" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B143" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C143" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D143" s="4" t="n">
         <v>43465</v>
@@ -13321,14 +13317,14 @@
     </row>
     <row r="144" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B144" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C144" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D144" s="4" t="n">
         <v>43465</v>
@@ -13411,14 +13407,14 @@
     </row>
     <row r="145" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B145" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C145" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D145" s="4" t="n">
         <v>43465</v>
@@ -13501,14 +13497,14 @@
     </row>
     <row r="146" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B146" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C146" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D146" s="4" t="n">
         <v>43465</v>
@@ -13591,14 +13587,14 @@
     </row>
     <row r="147" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C147" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D147" s="4" t="n">
         <v>43465</v>
@@ -13681,14 +13677,14 @@
     </row>
     <row r="148" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C148" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D148" s="4" t="n">
         <v>43465</v>
@@ -13771,14 +13767,14 @@
     </row>
     <row r="149" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B149" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C149" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D149" s="4" t="n">
         <v>43465</v>
@@ -13861,14 +13857,14 @@
     </row>
     <row r="150" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B150" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C150" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D150" s="4" t="n">
         <v>43465</v>
@@ -13951,14 +13947,14 @@
     </row>
     <row r="151" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B151" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C151" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D151" s="4" t="n">
         <v>43465</v>
@@ -14041,14 +14037,14 @@
     </row>
     <row r="152" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B152" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C152" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D152" s="4" t="n">
         <v>43465</v>
@@ -14131,14 +14127,14 @@
     </row>
     <row r="153" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B153" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C153" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D153" s="4" t="n">
         <v>43465</v>
@@ -14156,7 +14152,7 @@
         <v>31</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J153" s="3" t="s">
         <v>47</v>
@@ -14221,14 +14217,14 @@
     </row>
     <row r="154" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B154" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C154" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D154" s="4" t="n">
         <v>43465</v>
@@ -14311,14 +14307,14 @@
     </row>
     <row r="155" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B155" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C155" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D155" s="4" t="n">
         <v>43465</v>
@@ -14401,14 +14397,14 @@
     </row>
     <row r="156" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B156" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C156" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D156" s="4" t="n">
         <v>43465</v>
@@ -14426,10 +14422,10 @@
         <v>31</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J156" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K156" s="3" t="s">
         <v>34</v>
@@ -14491,14 +14487,14 @@
     </row>
     <row r="157" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B157" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C157" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D157" s="4" t="n">
         <v>43465</v>
@@ -14581,14 +14577,14 @@
     </row>
     <row r="158" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C158" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D158" s="4" t="n">
         <v>43465</v>
@@ -14671,14 +14667,14 @@
     </row>
     <row r="159" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C159" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D159" s="4" t="n">
         <v>43465</v>
@@ -14761,14 +14757,14 @@
     </row>
     <row r="160" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C160" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D160" s="4" t="n">
         <v>43465</v>
@@ -14851,14 +14847,14 @@
     </row>
     <row r="161" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C161" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D161" s="4" t="n">
         <v>43465</v>
@@ -14941,14 +14937,14 @@
     </row>
     <row r="162" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C162" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D162" s="4" t="n">
         <v>43465</v>
@@ -15031,14 +15027,14 @@
     </row>
     <row r="163" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C163" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D163" s="4" t="n">
         <v>43465</v>
@@ -15121,14 +15117,14 @@
     </row>
     <row r="164" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B164" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C164" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D164" s="4" t="n">
         <v>43465</v>
@@ -15211,14 +15207,14 @@
     </row>
     <row r="165" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B165" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C165" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D165" s="4" t="n">
         <v>43465</v>
@@ -15301,14 +15297,14 @@
     </row>
     <row r="166" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C166" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D166" s="4" t="n">
         <v>43465</v>
@@ -15391,14 +15387,14 @@
     </row>
     <row r="167" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B167" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C167" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D167" s="4" t="n">
         <v>43465</v>
@@ -15481,14 +15477,14 @@
     </row>
     <row r="168" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C168" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D168" s="4" t="n">
         <v>43465</v>
@@ -15571,14 +15567,14 @@
     </row>
     <row r="169" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B169" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C169" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D169" s="4" t="n">
         <v>43465</v>
@@ -15661,14 +15657,14 @@
     </row>
     <row r="170" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C170" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D170" s="4" t="n">
         <v>43465</v>
@@ -15751,14 +15747,14 @@
     </row>
     <row r="171" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C171" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D171" s="4" t="n">
         <v>43465</v>
@@ -15776,10 +15772,10 @@
         <v>31</v>
       </c>
       <c r="I171" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J171" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K171" s="3" t="s">
         <v>34</v>
@@ -15841,14 +15837,14 @@
     </row>
     <row r="172" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C172" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D172" s="4" t="n">
         <v>43465</v>
@@ -15866,10 +15862,10 @@
         <v>31</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J172" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K172" s="3" t="s">
         <v>34</v>
@@ -15930,15 +15926,15 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="6" t="s">
-        <v>78</v>
+      <c r="A173" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C173" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D173" s="4" t="n">
         <v>43465</v>
@@ -16020,15 +16016,15 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="6" t="s">
-        <v>78</v>
+      <c r="A174" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C174" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D174" s="4" t="n">
         <v>43465</v>
@@ -16110,15 +16106,15 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="6" t="s">
-        <v>78</v>
+      <c r="A175" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C175" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D175" s="4" t="n">
         <v>43465</v>
@@ -16200,15 +16196,15 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="6" t="s">
-        <v>78</v>
+      <c r="A176" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C176" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D176" s="4" t="n">
         <v>43465</v>
@@ -16290,15 +16286,15 @@
       </c>
     </row>
     <row r="177" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="6" t="s">
-        <v>78</v>
+      <c r="A177" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B177" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C177" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D177" s="4" t="n">
         <v>43465</v>
@@ -16380,15 +16376,15 @@
       </c>
     </row>
     <row r="178" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="6" t="s">
-        <v>78</v>
+      <c r="A178" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C178" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D178" s="4" t="n">
         <v>43465</v>
@@ -16470,15 +16466,15 @@
       </c>
     </row>
     <row r="179" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="6" t="s">
-        <v>78</v>
+      <c r="A179" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B179" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C179" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D179" s="4" t="n">
         <v>43465</v>
@@ -16560,15 +16556,15 @@
       </c>
     </row>
     <row r="180" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="6" t="s">
-        <v>78</v>
+      <c r="A180" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C180" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D180" s="4" t="n">
         <v>43465</v>
@@ -16650,15 +16646,15 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="6" t="s">
-        <v>78</v>
+      <c r="A181" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B181" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C181" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D181" s="4" t="n">
         <v>43465</v>
@@ -16740,15 +16736,15 @@
       </c>
     </row>
     <row r="182" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="6" t="s">
-        <v>78</v>
+      <c r="A182" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C182" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D182" s="4" t="n">
         <v>43465</v>
@@ -16830,15 +16826,15 @@
       </c>
     </row>
     <row r="183" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="6" t="s">
-        <v>78</v>
+      <c r="A183" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B183" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C183" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D183" s="4" t="n">
         <v>43465</v>
@@ -16920,15 +16916,15 @@
       </c>
     </row>
     <row r="184" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="6" t="s">
-        <v>78</v>
+      <c r="A184" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C184" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D184" s="4" t="n">
         <v>43465</v>
@@ -17010,15 +17006,15 @@
       </c>
     </row>
     <row r="185" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="6" t="s">
-        <v>78</v>
+      <c r="A185" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B185" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C185" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D185" s="4" t="n">
         <v>43465</v>
@@ -17100,15 +17096,15 @@
       </c>
     </row>
     <row r="186" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="6" t="s">
-        <v>78</v>
+      <c r="A186" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C186" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D186" s="4" t="n">
         <v>43465</v>
@@ -17190,15 +17186,15 @@
       </c>
     </row>
     <row r="187" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="6" t="s">
-        <v>78</v>
+      <c r="A187" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B187" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C187" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D187" s="4" t="n">
         <v>43465</v>
@@ -17216,7 +17212,7 @@
         <v>31</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J187" s="3" t="s">
         <v>47</v>
@@ -17280,15 +17276,15 @@
       </c>
     </row>
     <row r="188" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="6" t="s">
-        <v>78</v>
+      <c r="A188" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B188" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C188" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D188" s="4" t="n">
         <v>43465</v>
@@ -17370,15 +17366,15 @@
       </c>
     </row>
     <row r="189" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="6" t="s">
-        <v>78</v>
+      <c r="A189" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B189" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C189" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D189" s="4" t="n">
         <v>43465</v>
@@ -17460,15 +17456,15 @@
       </c>
     </row>
     <row r="190" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="6" t="s">
-        <v>78</v>
+      <c r="A190" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C190" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D190" s="4" t="n">
         <v>43465</v>
@@ -17486,10 +17482,10 @@
         <v>31</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J190" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K190" s="3" t="s">
         <v>34</v>
@@ -17550,15 +17546,15 @@
       </c>
     </row>
     <row r="191" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="6" t="s">
-        <v>78</v>
+      <c r="A191" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B191" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C191" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D191" s="4" t="n">
         <v>43465</v>
@@ -17640,15 +17636,15 @@
       </c>
     </row>
     <row r="192" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="6" t="s">
-        <v>78</v>
+      <c r="A192" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C192" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D192" s="4" t="n">
         <v>43465</v>
@@ -17731,14 +17727,14 @@
     </row>
     <row r="193" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B193" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C193" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D193" s="4" t="n">
         <v>43465</v>
@@ -17821,14 +17817,14 @@
     </row>
     <row r="194" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C194" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D194" s="4" t="n">
         <v>43465</v>
@@ -17911,14 +17907,14 @@
     </row>
     <row r="195" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B195" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C195" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D195" s="4" t="n">
         <v>43465</v>
@@ -18001,14 +17997,14 @@
     </row>
     <row r="196" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C196" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D196" s="4" t="n">
         <v>43465</v>
@@ -18091,14 +18087,14 @@
     </row>
     <row r="197" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C197" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D197" s="4" t="n">
         <v>43465</v>
@@ -18181,14 +18177,14 @@
     </row>
     <row r="198" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C198" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D198" s="4" t="n">
         <v>43465</v>
@@ -18271,14 +18267,14 @@
     </row>
     <row r="199" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B199" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C199" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D199" s="4" t="n">
         <v>43465</v>
@@ -18296,7 +18292,7 @@
         <v>31</v>
       </c>
       <c r="I199" s="3" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J199" s="3" t="s">
         <v>47</v>
@@ -18361,14 +18357,14 @@
     </row>
     <row r="200" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C200" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D200" s="4" t="n">
         <v>43465</v>
@@ -18451,14 +18447,14 @@
     </row>
     <row r="201" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B201" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C201" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D201" s="4" t="n">
         <v>43465</v>
@@ -18541,14 +18537,14 @@
     </row>
     <row r="202" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C202" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D202" s="4" t="n">
         <v>43465</v>
@@ -18566,10 +18562,10 @@
         <v>31</v>
       </c>
       <c r="I202" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J202" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K202" s="3" t="s">
         <v>34</v>
@@ -18631,14 +18627,14 @@
     </row>
     <row r="203" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B203" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C203" s="4" t="n">
         <f aca="true">TODAY()</f>
-        <v>43424</v>
+        <v>43425</v>
       </c>
       <c r="D203" s="4" t="n">
         <v>43465</v>
@@ -18656,10 +18652,10 @@
         <v>31</v>
       </c>
       <c r="I203" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J203" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K203" s="3" t="s">
         <v>34</v>

</xml_diff>